<commit_message>
Ben Update - July 16th
Adding more data - EM Bonds, USD/JPY, VIX
</commit_message>
<xml_diff>
--- a/Dev/Ben/DataSource.xlsx
+++ b/Dev/Ben/DataSource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3378e7d37fbb753c/Documents/GitHub/Market_Indicator_Machine_Learning/Dev/Ben/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{0590C5C7-C802-475F-8933-81F9B66D679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46C448FE-7C70-4F22-8AA2-82025FC7C08F}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{0590C5C7-C802-475F-8933-81F9B66D679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61042AEE-EB8E-4DB1-B4E8-086265205F2E}"/>
   <bookViews>
     <workbookView xWindow="50100" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{F7975433-FC8D-4B90-B5FB-B03348EED385}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t xml:space="preserve">Data </t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t xml:space="preserve">Data Starting Point - Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not added to analysis </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Can start in 99 ?</t>
   </si>
 </sst>
 </file>
@@ -143,12 +155,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -163,11 +181,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04DA68-87E4-4B4A-8482-A7C29A0F972C}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,9 +515,10 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +537,11 @@
       <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -537,42 +560,51 @@
       <c r="F2" s="3">
         <v>35682</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -592,7 +624,7 @@
         <v>35430</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -611,8 +643,11 @@
       <c r="F6" s="3">
         <v>36160</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -629,7 +664,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -649,7 +684,7 @@
         <v>32875</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -666,7 +701,7 @@
         <v>25937</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -686,7 +721,7 @@
         <v>32875</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Ben - Push July 23rd
Include draft ppt (just the start) and additional notebooks
</commit_message>
<xml_diff>
--- a/Dev/Ben/DataSource.xlsx
+++ b/Dev/Ben/DataSource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3378e7d37fbb753c/Documents/GitHub/Market_Indicator_Machine_Learning/Dev/Ben/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{0590C5C7-C802-475F-8933-81F9B66D679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61042AEE-EB8E-4DB1-B4E8-086265205F2E}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{0590C5C7-C802-475F-8933-81F9B66D679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22DD303E-CBFB-4484-A443-75B42A69CB19}"/>
   <bookViews>
-    <workbookView xWindow="50100" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{F7975433-FC8D-4B90-B5FB-B03348EED385}"/>
+    <workbookView xWindow="53910" yWindow="1440" windowWidth="21945" windowHeight="12585" xr2:uid="{F7975433-FC8D-4B90-B5FB-B03348EED385}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSource" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t xml:space="preserve">Data </t>
   </si>
@@ -68,42 +68,15 @@
     <t>CSV</t>
   </si>
   <si>
-    <t>Ticker</t>
-  </si>
-  <si>
     <t>EM High Yield Bond Yields</t>
   </si>
   <si>
-    <t>ML/EMHYY</t>
-  </si>
-  <si>
-    <t>ML/BBBEY</t>
-  </si>
-  <si>
-    <t>ML/AAAEY</t>
-  </si>
-  <si>
-    <t>AAA Bond Yields</t>
-  </si>
-  <si>
-    <t>BBB Bond Yields</t>
-  </si>
-  <si>
     <t xml:space="preserve">SP500 Index </t>
   </si>
   <si>
-    <t>ML/BEY</t>
-  </si>
-  <si>
     <t xml:space="preserve">UST Yield Curve </t>
   </si>
   <si>
-    <t>USTREASURY/YIELD</t>
-  </si>
-  <si>
-    <t>CHRIS/CME_ES2</t>
-  </si>
-  <si>
     <t>USD/JPY FX Rate</t>
   </si>
   <si>
@@ -119,26 +92,65 @@
     <t>St Louis Fed</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Starting Point - Date </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not added to analysis </t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Can start in 99 ?</t>
+    <t>USD LIBOR 3M</t>
+  </si>
+  <si>
+    <t>JPY LIBOR 3M</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>SP500 Open Price (t)</t>
+  </si>
+  <si>
+    <t>SP500 Close Price (t)</t>
+  </si>
+  <si>
+    <t>SP500_10_day_Moving_Average</t>
+  </si>
+  <si>
+    <t>SP500_10_day_Volatility_Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature Engineering </t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>10_day_Rolling_mean</t>
+  </si>
+  <si>
+    <t>10_day_Rolling_std</t>
+  </si>
+  <si>
+    <t>SP500_10_day_Correlation</t>
+  </si>
+  <si>
+    <t>Open_Price(t) - Close_Price(t)</t>
+  </si>
+  <si>
+    <t>10_day_Rolling_corr</t>
+  </si>
+  <si>
+    <t>Open_Price(t) - Open_Price(t-1)</t>
+  </si>
+  <si>
+    <t>US 10 Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +166,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -164,12 +191,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -177,16 +204,167 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,241 +679,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04DA68-87E4-4B4A-8482-A7C29A0F972C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="35.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="G9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3">
-        <v>35682</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3">
-        <v>35430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3">
-        <v>36160</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="3">
-        <v>32875</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3">
-        <v>25937</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="G11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F10" s="3">
-        <v>32875</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3">
-        <v>18034</v>
+      <c r="H11" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ben - Push July 24th
Added graphs to the notebook + proper confusion matrix and metrics
</commit_message>
<xml_diff>
--- a/Dev/Ben/DataSource.xlsx
+++ b/Dev/Ben/DataSource.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3378e7d37fbb753c/Documents/GitHub/Market_Indicator_Machine_Learning/Dev/Ben/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{0590C5C7-C802-475F-8933-81F9B66D679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22DD303E-CBFB-4484-A443-75B42A69CB19}"/>
+  <xr:revisionPtr revIDLastSave="422" documentId="8_{0590C5C7-C802-475F-8933-81F9B66D679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F95C132-1BA2-42AF-9461-6E1C7BAE6786}"/>
   <bookViews>
-    <workbookView xWindow="53910" yWindow="1440" windowWidth="21945" windowHeight="12585" xr2:uid="{F7975433-FC8D-4B90-B5FB-B03348EED385}"/>
+    <workbookView xWindow="50100" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{F7975433-FC8D-4B90-B5FB-B03348EED385}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSource" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="149">
   <si>
     <t xml:space="preserve">Data </t>
   </si>
@@ -144,13 +145,349 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Feature Engineering</t>
+  </si>
+  <si>
+    <t>2Y</t>
+  </si>
+  <si>
+    <t>5Y</t>
+  </si>
+  <si>
+    <t>10Y</t>
+  </si>
+  <si>
+    <t>2s5s</t>
+  </si>
+  <si>
+    <t>5s10s</t>
+  </si>
+  <si>
+    <t>2s10s</t>
+  </si>
+  <si>
+    <t>2s5s_20-day_Vol</t>
+  </si>
+  <si>
+    <t>5s10s_20-day_Vol</t>
+  </si>
+  <si>
+    <t>2s10s_20-day_Vol</t>
+  </si>
+  <si>
+    <t>2s5s_21-day_MA</t>
+  </si>
+  <si>
+    <t>Credit_55-day_MA</t>
+  </si>
+  <si>
+    <t>Credit_100-day_MA</t>
+  </si>
+  <si>
+    <t>Nikkei_Returns</t>
+  </si>
+  <si>
+    <t>Nikkei_20-day_Vol</t>
+  </si>
+  <si>
+    <t>Nikkei_50-day_Vol</t>
+  </si>
+  <si>
+    <t>Nikkei_100-day_Vol</t>
+  </si>
+  <si>
+    <t>Nikkei_21-day_MA</t>
+  </si>
+  <si>
+    <t>Nikkei_55-day_MA</t>
+  </si>
+  <si>
+    <t>Nikkei_100-day_MA</t>
+  </si>
+  <si>
+    <t>2s5s_55-day_MA</t>
+  </si>
+  <si>
+    <t>2s5s_100-day_MA</t>
+  </si>
+  <si>
+    <t>5s10s_21-day_MA</t>
+  </si>
+  <si>
+    <t>5s10s_55-day_MA</t>
+  </si>
+  <si>
+    <t>5s10s_100-day_MA</t>
+  </si>
+  <si>
+    <t>2s10s_21-day_MA</t>
+  </si>
+  <si>
+    <t>2s10s_55-day_MA</t>
+  </si>
+  <si>
+    <t>2s10s_100-day_MA</t>
+  </si>
+  <si>
+    <t>Closing_Price</t>
+  </si>
+  <si>
+    <t>SP500_Daily_Return</t>
+  </si>
+  <si>
+    <t>SP500_20-day_Vol</t>
+  </si>
+  <si>
+    <t>SP500_50-day_Vol</t>
+  </si>
+  <si>
+    <t>SP500_100-day_Vol</t>
+  </si>
+  <si>
+    <t>SP500_21-day_MA</t>
+  </si>
+  <si>
+    <t>SP500_55-day_MA</t>
+  </si>
+  <si>
+    <t>SP500_100-day_MA</t>
+  </si>
+  <si>
+    <t>EM_High_Yield</t>
+  </si>
+  <si>
+    <t>EM_Bonds_20-day_Vol</t>
+  </si>
+  <si>
+    <t>EM_Bonds_50-day_Vol</t>
+  </si>
+  <si>
+    <t>EM_Bonds_100-day_Vol</t>
+  </si>
+  <si>
+    <t>EM_Bonds_21-day_MA</t>
+  </si>
+  <si>
+    <t>EM_Bonds_55-day_MA</t>
+  </si>
+  <si>
+    <t>EM_Bonds_100-day_MA</t>
+  </si>
+  <si>
+    <t>USDJPY</t>
+  </si>
+  <si>
+    <t>USDJPY_21-day_MA</t>
+  </si>
+  <si>
+    <t>USDJPY_55-day_MA</t>
+  </si>
+  <si>
+    <t>USDJPY_100-day_MA</t>
+  </si>
+  <si>
+    <t>Ted_Spread</t>
+  </si>
+  <si>
+    <t>B_Spread</t>
+  </si>
+  <si>
+    <t>Five_year</t>
+  </si>
+  <si>
+    <t>B_UST_Spread</t>
+  </si>
+  <si>
+    <t>Credit_21-day_MA</t>
+  </si>
+  <si>
+    <t>VIX_55-day_MA</t>
+  </si>
+  <si>
+    <t>VIX_21-day_MA</t>
+  </si>
+  <si>
+    <t>VIX_100-day_MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RATES </t>
+  </si>
+  <si>
+    <t>EQUITY</t>
+  </si>
+  <si>
+    <t>VOL</t>
+  </si>
+  <si>
+    <t>CREDIT</t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2s5s 21 day rolling mean </t>
+  </si>
+  <si>
+    <t>2s10s 20 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>5s10s 20 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>2s5s 20 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2s5s 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2s5s 100 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5s10s 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5s10s 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5s10s 100 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2s10s 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2s10s 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2s10s 100 day rolling mean </t>
+  </si>
+  <si>
+    <t>SP500 20 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>SP500 50 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>SP500 100 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP500 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP500 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP500 100 day rolling mean </t>
+  </si>
+  <si>
+    <t>Log Nikkei Close(t) / Log Nikkei Close(t-1)</t>
+  </si>
+  <si>
+    <t>Log SP500 Close(t) / Log SP500 Close(t-1)</t>
+  </si>
+  <si>
+    <t>Nikkei 20 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>Nikkei 50 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>Nikkei 100 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikkei 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikkei 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikkei 100 day rolling mean </t>
+  </si>
+  <si>
+    <t>EM 20 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>EM 50 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t>EM 100 day rolling std (Returns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EM 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EM 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EM 100 day rolling mean </t>
+  </si>
+  <si>
+    <t>Diff(B Spread, 5Year UST)</t>
+  </si>
+  <si>
+    <t>Diff(5Yr, 2Yr)</t>
+  </si>
+  <si>
+    <t>Diff(10Yr, 5Yr)</t>
+  </si>
+  <si>
+    <t>Diff(10Yr, 2Yr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit 100 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIX 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIX 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIX 100 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD/JPY 21 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD/JPY 55 day rolling mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD/JPY 100 day rolling mean </t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>• 2s5s 21day MA</t>
+  </si>
+  <si>
+    <t>• 5s10s Curve                • 2s5s 55day MA</t>
+  </si>
+  <si>
+    <t>• 2s10s Curve                •  2s5s 100day MA</t>
+  </si>
+  <si>
+    <t>• 2s10s 20day Vol         •  5s10s 21day MA</t>
+  </si>
+  <si>
+    <t>• 5s10s 20day Vol         •  5s10s 55day MA</t>
+  </si>
+  <si>
+    <t>• 2s5s 20day Vol            • 5s10s 100day MA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +518,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF203864"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +586,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FAADC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EBF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -339,11 +754,180 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -359,11 +943,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04DA68-87E4-4B4A-8482-A7C29A0F972C}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +1344,7 @@
     <col min="8" max="8" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -708,7 +1359,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -722,17 +1373,8 @@
         <v>8</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -746,17 +1388,8 @@
         <v>8</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -770,17 +1403,8 @@
         <v>8</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -793,17 +1417,8 @@
       <c r="D5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -817,17 +1432,8 @@
         <v>8</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -840,17 +1446,8 @@
       <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -863,17 +1460,8 @@
       <c r="D8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -886,17 +1474,8 @@
       <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -909,17 +1488,8 @@
       <c r="D10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
@@ -931,19 +1501,1087 @@
       </c>
       <c r="D11" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60670B24-FAB1-486C-A442-BB94F622B020}">
+  <dimension ref="A1:CO70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="2"/>
+    <col min="13" max="14" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="24.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="23" style="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="24.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26" style="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="72" max="93" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:73" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+    </row>
+    <row r="2" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+    </row>
+    <row r="3" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="43"/>
+      <c r="B3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+    </row>
+    <row r="4" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="43"/>
+      <c r="B4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+    </row>
+    <row r="5" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="43"/>
+      <c r="B5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="43"/>
+      <c r="B7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+    </row>
+    <row r="8" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="43"/>
+      <c r="B8" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="43"/>
+      <c r="B9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="43"/>
+      <c r="B10" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+    </row>
+    <row r="11" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+    </row>
+    <row r="12" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="43"/>
+      <c r="B12" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="43"/>
+      <c r="B13" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="43"/>
+      <c r="B14" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:73" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="43"/>
+      <c r="B16" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="43"/>
+      <c r="B17" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="43"/>
+      <c r="B18" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="43"/>
+      <c r="B19" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="44"/>
+      <c r="B20" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="43"/>
+      <c r="B22" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="43"/>
+      <c r="B24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="43"/>
+      <c r="B25" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="43"/>
+      <c r="B28" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="43"/>
+      <c r="B30" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="43"/>
+      <c r="B31" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="43"/>
+      <c r="B32" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="43"/>
+      <c r="B33" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="43"/>
+      <c r="B35" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="43"/>
+      <c r="B36" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="43"/>
+      <c r="B38" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="43"/>
+      <c r="B39" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="43"/>
+      <c r="B40" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="43"/>
+      <c r="B41" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="43"/>
+      <c r="B42" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="43"/>
+      <c r="B43" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="43"/>
+      <c r="B44" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="43"/>
+      <c r="B45" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="43"/>
+      <c r="B46" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="43"/>
+      <c r="B47" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="43"/>
+      <c r="B48" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="44"/>
+      <c r="B49" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="43"/>
+      <c r="B51" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="43"/>
+      <c r="B52" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="44"/>
+      <c r="B53" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="43"/>
+      <c r="B55" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="43"/>
+      <c r="B56" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="44"/>
+      <c r="B57" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A21:A36"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A37:A49"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A2:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>